<commit_message>
Clases de ryp hechas
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p7/P6_UO277876.xlsx
+++ b/src/main/java/algestudiante/p7/P6_UO277876.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E61B29-2BE9-418B-A8AA-90EFC5923311}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAC24E0-4B31-439C-8AEF-2A89299D7246}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
+    <workbookView xWindow="9444" yWindow="768" windowWidth="10764" windowHeight="9480" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Ramifica y poda" sheetId="5" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Complejidad:</t>
   </si>
   <si>
-    <t>O(n!)</t>
-  </si>
-  <si>
     <t>nVeces = 100</t>
   </si>
   <si>
@@ -73,6 +70,9 @@
   </si>
   <si>
     <t>nVeces (ryp)</t>
+  </si>
+  <si>
+    <t>O(3^n)</t>
   </si>
 </sst>
 </file>
@@ -1555,7 +1555,7 @@
   <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1574,10 +1574,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>1</v>
@@ -1596,7 +1596,7 @@
         <v>1.3299999999999999E-2</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>2</v>
@@ -1615,7 +1615,7 @@
         <v>2.0819999999999999</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>3</v>
@@ -1634,7 +1634,7 @@
         <v>525.6</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="2">
         <v>10000000</v>
@@ -1645,7 +1645,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="20"/>
       <c r="I6" s="2">
@@ -1657,7 +1657,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="I7" s="3">
         <v>100000</v>

</xml_diff>